<commit_message>
Trial check for tfs send screenshot error
</commit_message>
<xml_diff>
--- a/docs/tp/Clients_FE_TP.xlsx
+++ b/docs/tp/Clients_FE_TP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TA\matrix-web-fe-tests\docs\tp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10658FB9-C79B-440F-8107-A9F4F633C888}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE224DD5-E7AC-41DD-A015-839A52D34A89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="28920" windowHeight="15900" xr2:uid="{BE46A6EB-3E52-4087-BE1D-BF4A8643FA88}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="68">
   <si>
     <t>Oboe Andrea (Leased Employee)</t>
   </si>
@@ -210,6 +210,33 @@
   </si>
   <si>
     <t xml:space="preserve">Verificre che l'unico venga stampato correttamente </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accedere a MW e Ricercare un cliente </t>
+  </si>
+  <si>
+    <t>Verificare il caricamento corretto della scheda del cliente</t>
+  </si>
+  <si>
+    <t>Modifica cliente PG (1)</t>
+  </si>
+  <si>
+    <t>Modifica cliente PG (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accedere alla modifica e modificare alcuni dati inserendo la PEC il consenso all'invio PEC portare a termine la modifica </t>
+  </si>
+  <si>
+    <t>Verificare che venga richiesto il caricamento del documento d'identità e caricalo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nella Customer View </t>
+  </si>
+  <si>
+    <t>Modifica cliente PG (3)</t>
+  </si>
+  <si>
+    <t>Verificare che i consensi/contatti si siano aggiornati correttamente - verificare il folder (unici + documento)</t>
   </si>
 </sst>
 </file>
@@ -311,7 +338,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -327,6 +354,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -642,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AEFEBA-728D-4FDD-9B3D-F6BE0E3793BC}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1154,8 +1184,95 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34" s="6"/>
+    <row r="18" spans="1:9" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="7" customFormat="1" ht="42" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="7" customFormat="1" ht="42" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C32" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>